<commit_message>
Reorganized codes, made general fd model, added n2
</commit_message>
<xml_diff>
--- a/Juan_Work/comparing model-vital pathways.xlsx
+++ b/Juan_Work/comparing model-vital pathways.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="72" windowWidth="9672" windowHeight="6036"/>
+    <workbookView xWindow="480" yWindow="72" windowWidth="9672" windowHeight="6036" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Catabolic" sheetId="1" r:id="rId1"/>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1418,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>

</xml_diff>